<commit_message>
Type correction for self-attention
</commit_message>
<xml_diff>
--- a/Transformers/img/tables.xlsx
+++ b/Transformers/img/tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alex/Projects_mix/teaching_content/Transformers/img/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF84BC05-9307-AD44-B446-75DFB49C1865}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93C1768E-DBAB-674D-8376-20C2557240AC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2920" yWindow="2300" windowWidth="25100" windowHeight="15700" xr2:uid="{8FF7F3CF-775C-0C44-A0FB-888F58045653}"/>
   </bookViews>
@@ -212,9 +212,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -233,6 +230,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -551,8 +551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52C51B5F-EC43-EF4D-B509-AFA3707B82CB}">
   <dimension ref="C6:AK18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="117" workbookViewId="0">
-      <selection activeCell="AH14" sqref="AH14"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="S1" zoomScale="117" workbookViewId="0">
+      <selection activeCell="Z16" sqref="Z16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -564,24 +564,24 @@
     <col min="14" max="18" width="3.33203125" customWidth="1"/>
     <col min="20" max="24" width="5.83203125" customWidth="1"/>
     <col min="26" max="30" width="5.83203125" style="3" customWidth="1"/>
-    <col min="31" max="31" width="17.6640625" customWidth="1"/>
+    <col min="31" max="31" width="18.33203125" customWidth="1"/>
     <col min="32" max="36" width="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="6" spans="3:37" x14ac:dyDescent="0.2">
-      <c r="AF6" s="23" t="s">
+      <c r="AF6" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="AG6" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="AH6" s="23" t="s">
+      <c r="AG6" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="AH6" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="AI6" s="23" t="s">
+      <c r="AI6" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="AJ6" s="23" t="s">
+      <c r="AJ6" s="22" t="s">
         <v>8</v>
       </c>
     </row>
@@ -619,47 +619,47 @@
       <c r="X7" s="14">
         <v>0</v>
       </c>
-      <c r="Z7" s="18">
-        <f>T7/SQRT(5)</f>
-        <v>12.969194269498779</v>
-      </c>
-      <c r="AA7" s="15">
-        <f>U7/SQRT(5)</f>
-        <v>0</v>
-      </c>
-      <c r="AB7" s="15">
-        <f>V7/SQRT(5)</f>
-        <v>4.4721359549995796</v>
-      </c>
-      <c r="AC7" s="15">
-        <f>W7/SQRT(5)</f>
-        <v>4.4721359549995796</v>
-      </c>
-      <c r="AD7" s="15">
-        <f>X7/SQRT(5)</f>
-        <v>0</v>
-      </c>
-      <c r="AF7" s="19">
+      <c r="Z7" s="17">
+        <f>T7/SQRT(3)</f>
+        <v>16.743157806499148</v>
+      </c>
+      <c r="AA7" s="23">
+        <f t="shared" ref="AA7:AD7" si="0">U7/SQRT(3)</f>
+        <v>0</v>
+      </c>
+      <c r="AB7" s="23">
+        <f t="shared" si="0"/>
+        <v>5.7735026918962582</v>
+      </c>
+      <c r="AC7" s="23">
+        <f t="shared" si="0"/>
+        <v>5.7735026918962582</v>
+      </c>
+      <c r="AD7" s="23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AF7" s="18">
         <f>EXP(Z7)/(EXP(Z7)+EXP(AB7)+EXP(AC7)+EXP(AA7)+EXP(AD7))</f>
-        <v>0.99958737266299025</v>
-      </c>
-      <c r="AG7" s="20">
+        <v>0.99996546158746358</v>
+      </c>
+      <c r="AG7" s="19">
         <f>EXP(AA7)/(EXP(Z7)+EXP(AB7)+EXP(AC7)+EXP(AA7)+EXP(AD7))</f>
-        <v>2.3300822700169269E-6</v>
-      </c>
-      <c r="AH7" s="20">
+        <v>5.3520967415834096E-8</v>
+      </c>
+      <c r="AH7" s="19">
         <f>EXP(AB7)/(EXP(Z7)+EXP(AB7)+EXP(AC7)+EXP(AA7)+EXP(AD7))</f>
-        <v>2.0398358623483002E-4</v>
-      </c>
-      <c r="AI7" s="20">
+        <v>1.7215685300818019E-5</v>
+      </c>
+      <c r="AI7" s="19">
         <f>EXP(AC7)/(EXP(Z7)+EXP(AB7)+EXP(AC7)+EXP(AA7)+EXP(AD7))</f>
-        <v>2.0398358623483002E-4</v>
-      </c>
-      <c r="AJ7" s="20">
+        <v>1.7215685300818019E-5</v>
+      </c>
+      <c r="AJ7" s="19">
         <f>EXP(AD7)/(EXP(Z7)+EXP(AB7)+EXP(AC7)+EXP(AA7)+EXP(AD7))</f>
-        <v>2.3300822700169269E-6</v>
-      </c>
-      <c r="AK7" s="22" t="s">
+        <v>5.3520967415834096E-8</v>
+      </c>
+      <c r="AK7" s="21" t="s">
         <v>4</v>
       </c>
     </row>
@@ -713,47 +713,47 @@
       <c r="X8" s="3">
         <v>30</v>
       </c>
-      <c r="Z8" s="15">
-        <f t="shared" ref="Z8:Z11" si="0">T8/SQRT(5)</f>
-        <v>0</v>
-      </c>
-      <c r="AA8" s="18">
-        <f t="shared" ref="AA8:AA11" si="1">U8/SQRT(5)</f>
-        <v>11.180339887498947</v>
-      </c>
-      <c r="AB8" s="15">
-        <f t="shared" ref="AB8:AB11" si="2">V8/SQRT(5)</f>
-        <v>0</v>
-      </c>
-      <c r="AC8" s="15">
-        <f t="shared" ref="AC8:AC11" si="3">W8/SQRT(5)</f>
-        <v>0</v>
-      </c>
-      <c r="AD8" s="15">
-        <f t="shared" ref="AD8:AD11" si="4">X8/SQRT(5)</f>
-        <v>13.416407864998737</v>
-      </c>
-      <c r="AF8" s="21">
-        <f t="shared" ref="AF8:AF11" si="5">EXP(Z8)/(EXP(Z8)+EXP(AB8)+EXP(AC8)+EXP(AA8)+EXP(AD8))</f>
-        <v>1.3465628120228262E-6</v>
-      </c>
-      <c r="AG8" s="19">
-        <f t="shared" ref="AG8:AG11" si="6">EXP(AA8)/(EXP(Z8)+EXP(AB8)+EXP(AC8)+EXP(AA8)+EXP(AD8))</f>
-        <v>9.6557616182561506E-2</v>
-      </c>
-      <c r="AH8" s="20">
-        <f t="shared" ref="AH8:AH11" si="7">EXP(AB8)/(EXP(Z8)+EXP(AB8)+EXP(AC8)+EXP(AA8)+EXP(AD8))</f>
-        <v>1.3465628120228262E-6</v>
-      </c>
-      <c r="AI8" s="20">
-        <f t="shared" ref="AI8:AI11" si="8">EXP(AC8)/(EXP(Z8)+EXP(AB8)+EXP(AC8)+EXP(AA8)+EXP(AD8))</f>
-        <v>1.3465628120228262E-6</v>
-      </c>
-      <c r="AJ8" s="20">
-        <f t="shared" ref="AJ8:AJ11" si="9">EXP(AD8)/(EXP(Z8)+EXP(AB8)+EXP(AC8)+EXP(AA8)+EXP(AD8))</f>
-        <v>0.90343834412900248</v>
-      </c>
-      <c r="AK8" s="22" t="s">
+      <c r="Z8" s="23">
+        <f t="shared" ref="Z8:Z11" si="1">T8/SQRT(3)</f>
+        <v>0</v>
+      </c>
+      <c r="AA8" s="17">
+        <f t="shared" ref="AA8:AA11" si="2">U8/SQRT(3)</f>
+        <v>14.433756729740645</v>
+      </c>
+      <c r="AB8" s="23">
+        <f t="shared" ref="AB8:AB11" si="3">V8/SQRT(3)</f>
+        <v>0</v>
+      </c>
+      <c r="AC8" s="23">
+        <f t="shared" ref="AC8:AC11" si="4">W8/SQRT(3)</f>
+        <v>0</v>
+      </c>
+      <c r="AD8" s="23">
+        <f t="shared" ref="AD8:AD11" si="5">X8/SQRT(3)</f>
+        <v>17.320508075688775</v>
+      </c>
+      <c r="AF8" s="20">
+        <f t="shared" ref="AF8:AF11" si="6">EXP(Z8)/(EXP(Z8)+EXP(AB8)+EXP(AC8)+EXP(AA8)+EXP(AD8))</f>
+        <v>2.8459999624852772E-8</v>
+      </c>
+      <c r="AG8" s="18">
+        <f t="shared" ref="AG8:AG11" si="7">EXP(AA8)/(EXP(Z8)+EXP(AB8)+EXP(AC8)+EXP(AA8)+EXP(AD8))</f>
+        <v>5.2812386249344985E-2</v>
+      </c>
+      <c r="AH8" s="19">
+        <f t="shared" ref="AH8:AH11" si="8">EXP(AB8)/(EXP(Z8)+EXP(AB8)+EXP(AC8)+EXP(AA8)+EXP(AD8))</f>
+        <v>2.8459999624852772E-8</v>
+      </c>
+      <c r="AI8" s="19">
+        <f t="shared" ref="AI8:AI11" si="9">EXP(AC8)/(EXP(Z8)+EXP(AB8)+EXP(AC8)+EXP(AA8)+EXP(AD8))</f>
+        <v>2.8459999624852772E-8</v>
+      </c>
+      <c r="AJ8" s="19">
+        <f t="shared" ref="AJ8:AJ11" si="10">EXP(AD8)/(EXP(Z8)+EXP(AB8)+EXP(AC8)+EXP(AA8)+EXP(AD8))</f>
+        <v>0.94718752837065623</v>
+      </c>
+      <c r="AK8" s="21" t="s">
         <v>5</v>
       </c>
     </row>
@@ -797,7 +797,7 @@
       <c r="R9" s="13">
         <v>0</v>
       </c>
-      <c r="S9" s="16" t="s">
+      <c r="S9" s="15" t="s">
         <v>13</v>
       </c>
       <c r="T9" s="3">
@@ -815,53 +815,53 @@
       <c r="X9" s="3">
         <v>0</v>
       </c>
-      <c r="Y9" s="17" t="s">
+      <c r="Y9" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="Z9" s="15">
-        <f t="shared" si="0"/>
-        <v>4.4721359549995796</v>
-      </c>
-      <c r="AA9" s="15">
+      <c r="Z9" s="23">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AB9" s="18">
+        <v>5.7735026918962582</v>
+      </c>
+      <c r="AA9" s="23">
         <f t="shared" si="2"/>
-        <v>11.180339887498947</v>
-      </c>
-      <c r="AC9" s="15">
+        <v>0</v>
+      </c>
+      <c r="AB9" s="17">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AD9" s="15">
+        <v>14.433756729740645</v>
+      </c>
+      <c r="AC9" s="23">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="AE9" s="16" t="s">
+      <c r="AD9" s="23">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AE9" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="AF9" s="21">
-        <f t="shared" si="5"/>
-        <v>1.2193152748181382E-3</v>
-      </c>
-      <c r="AG9" s="20">
+      <c r="AF9" s="20">
         <f t="shared" si="6"/>
-        <v>1.3928105470916778E-5</v>
-      </c>
-      <c r="AH9" s="19">
+        <v>1.7330994454588293E-4</v>
+      </c>
+      <c r="AG9" s="19">
         <f t="shared" si="7"/>
-        <v>0.998738900408769</v>
-      </c>
-      <c r="AI9" s="20">
+        <v>5.3879446172494041E-7</v>
+      </c>
+      <c r="AH9" s="18">
         <f t="shared" si="8"/>
-        <v>1.3928105470916778E-5</v>
-      </c>
-      <c r="AJ9" s="20">
+        <v>0.99982507367206896</v>
+      </c>
+      <c r="AI9" s="19">
         <f t="shared" si="9"/>
-        <v>1.3928105470916778E-5</v>
-      </c>
-      <c r="AK9" s="22" t="s">
+        <v>5.3879446172494041E-7</v>
+      </c>
+      <c r="AJ9" s="19">
+        <f t="shared" si="10"/>
+        <v>5.3879446172494041E-7</v>
+      </c>
+      <c r="AK9" s="21" t="s">
         <v>6</v>
       </c>
     </row>
@@ -920,47 +920,47 @@
       <c r="X10" s="3">
         <v>0</v>
       </c>
-      <c r="Z10" s="15">
-        <f t="shared" si="0"/>
-        <v>4.4721359549995796</v>
-      </c>
-      <c r="AA10" s="15">
+      <c r="Z10" s="23">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AB10" s="15">
+        <v>5.7735026918962582</v>
+      </c>
+      <c r="AA10" s="23">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AC10" s="18">
+      <c r="AB10" s="23">
         <f t="shared" si="3"/>
-        <v>1.7888543819998317</v>
-      </c>
-      <c r="AD10" s="15">
+        <v>0</v>
+      </c>
+      <c r="AC10" s="17">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="AF10" s="21">
+        <v>2.3094010767585034</v>
+      </c>
+      <c r="AD10" s="23">
         <f t="shared" si="5"/>
-        <v>0.90694129258332279</v>
-      </c>
-      <c r="AG10" s="20">
+        <v>0</v>
+      </c>
+      <c r="AF10" s="20">
         <f t="shared" si="6"/>
-        <v>1.0359891522653304E-2</v>
-      </c>
-      <c r="AH10" s="20">
+        <v>0.96095850415205963</v>
+      </c>
+      <c r="AG10" s="19">
         <f t="shared" si="7"/>
-        <v>1.0359891522653304E-2</v>
-      </c>
-      <c r="AI10" s="19">
+        <v>2.9874749619317937E-3</v>
+      </c>
+      <c r="AH10" s="19">
         <f t="shared" si="8"/>
-        <v>6.1979032848717287E-2</v>
-      </c>
-      <c r="AJ10" s="20">
+        <v>2.9874749619317937E-3</v>
+      </c>
+      <c r="AI10" s="18">
         <f t="shared" si="9"/>
-        <v>1.0359891522653304E-2</v>
-      </c>
-      <c r="AK10" s="22" t="s">
+        <v>3.0079070962144922E-2</v>
+      </c>
+      <c r="AJ10" s="19">
+        <f t="shared" si="10"/>
+        <v>2.9874749619317937E-3</v>
+      </c>
+      <c r="AK10" s="21" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1001,47 +1001,47 @@
       <c r="X11" s="3">
         <v>36</v>
       </c>
-      <c r="Z11" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AA11" s="15">
+      <c r="Z11" s="23">
         <f t="shared" si="1"/>
-        <v>13.416407864998737</v>
-      </c>
-      <c r="AB11" s="15">
+        <v>0</v>
+      </c>
+      <c r="AA11" s="23">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="AC11" s="15">
+        <v>17.320508075688775</v>
+      </c>
+      <c r="AB11" s="23">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AD11" s="18">
+      <c r="AC11" s="23">
         <f t="shared" si="4"/>
-        <v>16.099689437998485</v>
-      </c>
-      <c r="AF11" s="21">
+        <v>0</v>
+      </c>
+      <c r="AD11" s="17">
         <f t="shared" si="5"/>
-        <v>9.5342097419244571E-8</v>
-      </c>
-      <c r="AG11" s="20">
+        <v>20.784609690826528</v>
+      </c>
+      <c r="AF11" s="20">
         <f t="shared" si="6"/>
-        <v>6.3967091508218651E-2</v>
-      </c>
-      <c r="AH11" s="20">
+        <v>9.1195459310149687E-10</v>
+      </c>
+      <c r="AG11" s="19">
         <f t="shared" si="7"/>
-        <v>9.5342097419244571E-8</v>
-      </c>
-      <c r="AI11" s="20">
+        <v>3.0351090246387973E-2</v>
+      </c>
+      <c r="AH11" s="19">
         <f t="shared" si="8"/>
-        <v>9.5342097419244571E-8</v>
-      </c>
-      <c r="AJ11" s="19">
+        <v>9.1195459310149687E-10</v>
+      </c>
+      <c r="AI11" s="19">
         <f t="shared" si="9"/>
-        <v>0.93603262246548902</v>
-      </c>
-      <c r="AK11" s="22" t="s">
+        <v>9.1195459310149687E-10</v>
+      </c>
+      <c r="AJ11" s="18">
+        <f t="shared" si="10"/>
+        <v>0.9696489070177482</v>
+      </c>
+      <c r="AK11" s="21" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>